<commit_message>
implemented cllecting data from a given session
</commit_message>
<xml_diff>
--- a/sessionsData/sessionData2024-06-05.xlsx
+++ b/sessionsData/sessionData2024-06-05.xlsx
@@ -465,19 +465,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>115</v>
+        <v>28</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>30</v>
+        <v>2.5</v>
       </c>
       <c r="F2" t="n">
-        <v>6.5</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>